<commit_message>
fixed a lot of the styling
</commit_message>
<xml_diff>
--- a/participants.xlsx
+++ b/participants.xlsx
@@ -41,7 +41,7 @@
             <text:p>Email</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>Names</text:p>
+            <text:p>Name</text:p>
           </table:table-cell>
         </table:table-row>
         <table:table-row table:style-name="ro1">
@@ -52,6 +52,26 @@
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Marijn Borghoutys</text:p>
+          </table:table-cell>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>
+              <text:a xlink:href="mailto:marino@b.com" xlink:type="simple">marino@b.com</text:a>
+            </text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Marino b</text:p>
+          </table:table-cell>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>
+              <text:a xlink:href="mailto:Niek@muis.com" xlink:type="simple">Niek@muis.com</text:a>
+            </text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>niek muijs</text:p>
           </table:table-cell>
         </table:table-row>
       </table:table>
@@ -65,11 +85,11 @@
 <office:document-meta xmlns:office="urn:oasis:names:tc:opendocument:xmlns:office:1.0" xmlns:ooo="http://openoffice.org/2004/office" xmlns:xlink="http://www.w3.org/1999/xlink" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:meta="urn:oasis:names:tc:opendocument:xmlns:meta:1.0" xmlns:grddl="http://www.w3.org/2003/g/data-view#" office:version="1.3">
   <office:meta>
     <meta:creation-date>2024-09-25T17:19:04.165000000</meta:creation-date>
-    <dc:date>2024-09-25T17:20:33.913000000</dc:date>
-    <meta:editing-duration>PT1M30S</meta:editing-duration>
-    <meta:editing-cycles>1</meta:editing-cycles>
-    <meta:document-statistic meta:table-count="1" meta:cell-count="4" meta:object-count="0"/>
+    <dc:date>2024-09-25T19:22:50.067000000</dc:date>
+    <meta:editing-duration>PT2M39S</meta:editing-duration>
+    <meta:editing-cycles>5</meta:editing-cycles>
     <meta:generator>LibreOffice/24.8.0.3$Windows_X86_64 LibreOffice_project/0bdf1299c94fe897b119f97f3c613e9dca6be583</meta:generator>
+    <meta:document-statistic meta:table-count="1" meta:cell-count="8" meta:object-count="0"/>
   </office:meta>
 </office:document-meta>
 </file>
@@ -81,14 +101,14 @@
       <config:config-item config:name="VisibleAreaTop" config:type="int">0</config:config-item>
       <config:config-item config:name="VisibleAreaLeft" config:type="int">0</config:config-item>
       <config:config-item config:name="VisibleAreaWidth" config:type="int">4516</config:config-item>
-      <config:config-item config:name="VisibleAreaHeight" config:type="int">903</config:config-item>
+      <config:config-item config:name="VisibleAreaHeight" config:type="int">1806</config:config-item>
       <config:config-item-map-indexed config:name="Views">
         <config:config-item-map-entry>
           <config:config-item config:name="ViewId" config:type="string">view1</config:config-item>
           <config:config-item-map-named config:name="Tables">
             <config:config-item-map-entry config:name="Sheet1">
               <config:config-item config:name="CursorPositionX" config:type="int">1</config:config-item>
-              <config:config-item config:name="CursorPositionY" config:type="int">1</config:config-item>
+              <config:config-item config:name="CursorPositionY" config:type="int">3</config:config-item>
               <config:config-item config:name="ActiveSplitRange" config:type="short">2</config:config-item>
               <config:config-item config:name="PositionLeft" config:type="int">0</config:config-item>
               <config:config-item config:name="PositionRight" config:type="int">0</config:config-item>
@@ -156,9 +176,9 @@
       <config:config-item config:name="IsSnapToRaster" config:type="boolean">false</config:config-item>
       <config:config-item config:name="LinkUpdateMode" config:type="short">3</config:config-item>
       <config:config-item config:name="LoadReadonly" config:type="boolean">false</config:config-item>
-      <config:config-item config:name="PrinterName" config:type="string"/>
+      <config:config-item config:name="PrinterName" config:type="string">Microsoft Print to PDF</config:config-item>
       <config:config-item config:name="PrinterPaperFromSetup" config:type="boolean">false</config:config-item>
-      <config:config-item config:name="PrinterSetup" config:type="base64Binary"/>
+      <config:config-item config:name="PrinterSetup" config:type="base64Binary">ZBb+/01pY3Jvc29mdCBQcmludCB0byBQREYAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAATWljcm9zb2Z0IFByaW50IFRvIFBERgAAAAAAAAAAAAAWAAEANhUAAAAAAAAIAFZUAAAkbQAAM1ROVwAAAAAKAE0AaQBjAHIAbwBzAG8AZgB0ACAAUAByAGkAbgB0ACAAdABvACAAUABEAEYAAAAAAAAAAAAAAAAAAAAAAAAAAAABBAMG3ABQFAMvAQABAAEA6gpvCGQAAQAPAFgCAgABAFgCAwABAEwAZQB0AHQAZQByAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAEAAAAAAAAAAQAAAAIAAAABAAAA/////0dJUzQAAAAAAAAAAAAAAABESU5VIgDIACQDLBE/XXt+AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAUAAAAAAAkAAQAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAEAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAyAAAAFNNVEoAAAAAEAC4AHsAMAA4ADQARgAwADEARgBBAC0ARQA2ADMANAAtADQARAA3ADcALQA4ADMARQBFAC0AMAA3ADQAOAAxADcAQwAwADMANQA4ADEAfQAAAFJFU0RMTABVbmlyZXNETEwAUGFwZXJTaXplAExFVFRFUgBPcmllbnRhdGlvbgBQT1JUUkFJVABSZXNvbHV0aW9uAFJlc09wdGlvbjEAQ29sb3JNb2RlAENvbG9yAAAAAAAAAAAAAAAAAAAsEQAAVjRETQEAAAAAAAAAnApwIhwAAADsAAAAAwAAAPoBTwg05ndNg+4HSBfANYHQAAAATAAAAAMAAAAACAAAAAAAAAAAAAADAAAAAAgAACoAAAAACAAAAwAAAEAAAABWAAAAABAAAEQAbwBjAHUAbQBlAG4AdABVAHMAZQByAFAAYQBzAHMAdwBvAHIAZAAAAEQAbwBjAHUAbQBlAG4AdABPAHcAbgBlAHIAUABhAHMAcwB3AG8AcgBkAAAARABvAGMAdQBtAGUAbgB0AEMAcgB5AHAAdABTAGUAYwB1AHIAaQB0AHkAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAEgBDT01QQVRfRFVQTEVYX01PREUTAER1cGxleE1vZGU6OlVua25vd24MAFBSSU5URVJfTkFNRRYATWljcm9zb2Z0IFByaW50IHRvIFBERgsARFJJVkVSX05BTUUWAE1pY3Jvc29mdCBQcmludCBUbyBQREY=</config:config-item>
       <config:config-item config:name="RasterIsVisible" config:type="boolean">false</config:config-item>
       <config:config-item config:name="RasterResolutionX" config:type="int">1270</config:config-item>
       <config:config-item config:name="RasterResolutionY" config:type="int">1270</config:config-item>
@@ -172,6 +192,7 @@
       <config:config-item config:name="ShowNotes" config:type="boolean">true</config:config-item>
       <config:config-item config:name="ShowPageBreaks" config:type="boolean">true</config:config-item>
       <config:config-item config:name="ShowZeroValues" config:type="boolean">true</config:config-item>
+      <config:config-item config:name="SyntaxStringRef" config:type="short">7</config:config-item>
       <config:config-item config:name="UpdateFromTemplate" config:type="boolean">true</config:config-item>
       <config:config-item-map-named config:name="ScriptConfiguration">
         <config:config-item-map-entry config:name="Sheet1">
@@ -197,7 +218,7 @@
     </style:default-style>
     <style:default-style style:family="graphic">
       <style:graphic-properties svg:stroke-color="#3465a4" draw:fill-color="#729fcf" fo:wrap-option="no-wrap" draw:shadow-offset-x="0.1181in" draw:shadow-offset-y="0.1181in" style:writing-mode="page"/>
-      <style:paragraph-properties style:text-autospace="ideograph-alpha" style:punctuation-wrap="simple" style:line-break="strict" style:writing-mode="page" style:font-independent-line-spacing="false">
+      <style:paragraph-properties style:text-autospace="ideograph-alpha" style:punctuation-wrap="simple" style:line-break="strict" loext:tab-stop-distance="0in" style:writing-mode="page" style:font-independent-line-spacing="false">
         <style:tab-stops/>
       </style:paragraph-properties>
       <style:text-properties style:use-window-font-color="true" loext:opacity="0%" fo:font-family="'Liberation Serif'" style:font-family-generic="roman" style:font-pitch="variable" fo:font-size="12pt" fo:language="en" fo:country="US" style:letter-kerning="true" style:font-family-asian="'Segoe UI'" style:font-family-generic-asian="system" style:font-pitch-asian="variable" style:font-size-asian="12pt" style:language-asian="zh" style:country-asian="CN" style:font-family-complex="Tahoma" style:font-family-generic-complex="system" style:font-pitch-complex="variable" style:font-size-complex="12pt" style:language-complex="hi" style:country-complex="IN"/>
@@ -369,7 +390,7 @@
           <text:p>
             <text:date style:data-style-name="N2" text:date-value="2024-09-25">00/00/0000</text:date>
             , 
-            <text:time>00:00:00</text:time>
+            <text:time style:data-style-name="N2" text:time-value="19:22:22.826000000">00:00:00</text:time>
           </text:p>
         </style:region-right>
       </style:header>

</xml_diff>

<commit_message>
fixed some of the functionality
</commit_message>
<xml_diff>
--- a/participants.xlsx
+++ b/participants.xlsx
@@ -22,6 +22,12 @@
   </office:font-face-decls>
   <office:automatic-styles>
     <style:style style:name="co1" style:family="table-column">
+      <style:table-column-properties fo:break-before="auto" style:column-width="1.5209in"/>
+    </style:style>
+    <style:style style:name="co2" style:family="table-column">
+      <style:table-column-properties fo:break-before="auto" style:column-width="1.5791in"/>
+    </style:style>
+    <style:style style:name="co3" style:family="table-column">
       <style:table-column-properties fo:break-before="auto" style:column-width="0.889in"/>
     </style:style>
     <style:style style:name="ro1" style:family="table-row">
@@ -35,7 +41,8 @@
     <office:spreadsheet>
       <table:calculation-settings table:automatic-find-labels="false" table:use-regular-expressions="false" table:use-wildcards="true"/>
       <table:table table:name="Sheet1" table:style-name="ta1">
-        <table:table-column table:style-name="co1" table:number-columns-repeated="2" table:default-cell-style-name="Default"/>
+        <table:table-column table:style-name="co1" table:default-cell-style-name="Default"/>
+        <table:table-column table:style-name="co2" table:default-cell-style-name="Default"/>
         <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Email</text:p>
@@ -47,31 +54,21 @@
         <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>
-              <text:a xlink:href="mailto:marijnborghouts@gmail.com" xlink:type="simple">marijnborghouts@gmail.com</text:a>
+              <text:a xlink:href="mailto:m.f.a.peeters@student.tue.nl" xlink:type="simple">m.f.a.peeters@student.tue.nl</text:a>
             </text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>Marijn Borghoutys</text:p>
+            <text:p>Martijn Peeters</text:p>
           </table:table-cell>
         </table:table-row>
         <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>
-              <text:a xlink:href="mailto:marino@b.com" xlink:type="simple">marino@b.com</text:a>
+              <text:a xlink:href="mailto:m.m.borghouts@student.tue.nl" xlink:type="simple">m.m.borghouts@student.tue.nl</text:a>
             </text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>Marino b</text:p>
-          </table:table-cell>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>
-              <text:a xlink:href="mailto:Niek@muis.com" xlink:type="simple">Niek@muis.com</text:a>
-            </text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>niek muijs</text:p>
+            <text:p>Marijn Borghouts</text:p>
           </table:table-cell>
         </table:table-row>
       </table:table>
@@ -85,11 +82,11 @@
 <office:document-meta xmlns:office="urn:oasis:names:tc:opendocument:xmlns:office:1.0" xmlns:ooo="http://openoffice.org/2004/office" xmlns:xlink="http://www.w3.org/1999/xlink" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:meta="urn:oasis:names:tc:opendocument:xmlns:meta:1.0" xmlns:grddl="http://www.w3.org/2003/g/data-view#" office:version="1.3">
   <office:meta>
     <meta:creation-date>2024-09-25T17:19:04.165000000</meta:creation-date>
-    <dc:date>2024-09-25T19:22:50.067000000</dc:date>
-    <meta:editing-duration>PT2M39S</meta:editing-duration>
-    <meta:editing-cycles>5</meta:editing-cycles>
+    <dc:date>2024-09-25T20:54:47.147000000</dc:date>
+    <meta:editing-duration>PT4M8S</meta:editing-duration>
+    <meta:editing-cycles>7</meta:editing-cycles>
     <meta:generator>LibreOffice/24.8.0.3$Windows_X86_64 LibreOffice_project/0bdf1299c94fe897b119f97f3c613e9dca6be583</meta:generator>
-    <meta:document-statistic meta:table-count="1" meta:cell-count="8" meta:object-count="0"/>
+    <meta:document-statistic meta:table-count="1" meta:cell-count="6" meta:object-count="0"/>
   </office:meta>
 </office:document-meta>
 </file>
@@ -100,15 +97,15 @@
     <config:config-item-set config:name="ooo:view-settings">
       <config:config-item config:name="VisibleAreaTop" config:type="int">0</config:config-item>
       <config:config-item config:name="VisibleAreaLeft" config:type="int">0</config:config-item>
-      <config:config-item config:name="VisibleAreaWidth" config:type="int">4516</config:config-item>
-      <config:config-item config:name="VisibleAreaHeight" config:type="int">1806</config:config-item>
+      <config:config-item config:name="VisibleAreaWidth" config:type="int">7874</config:config-item>
+      <config:config-item config:name="VisibleAreaHeight" config:type="int">1355</config:config-item>
       <config:config-item-map-indexed config:name="Views">
         <config:config-item-map-entry>
           <config:config-item config:name="ViewId" config:type="string">view1</config:config-item>
           <config:config-item-map-named config:name="Tables">
             <config:config-item-map-entry config:name="Sheet1">
               <config:config-item config:name="CursorPositionX" config:type="int">1</config:config-item>
-              <config:config-item config:name="CursorPositionY" config:type="int">3</config:config-item>
+              <config:config-item config:name="CursorPositionY" config:type="int">2</config:config-item>
               <config:config-item config:name="ActiveSplitRange" config:type="short">2</config:config-item>
               <config:config-item config:name="PositionLeft" config:type="int">0</config:config-item>
               <config:config-item config:name="PositionRight" config:type="int">0</config:config-item>
@@ -390,7 +387,7 @@
           <text:p>
             <text:date style:data-style-name="N2" text:date-value="2024-09-25">00/00/0000</text:date>
             , 
-            <text:time style:data-style-name="N2" text:time-value="19:22:22.826000000">00:00:00</text:time>
+            <text:time style:data-style-name="N2" text:time-value="20:54:26.740000000">00:00:00</text:time>
           </text:p>
         </style:region-right>
       </style:header>

</xml_diff>